<commit_message>
team stuff, cleaner URLs
</commit_message>
<xml_diff>
--- a/team.xlsx
+++ b/team.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14128"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Curtis\Documents\GitHub\mcg\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18600" windowHeight="9735" tabRatio="500"/>
+    <workbookView xWindow="900" yWindow="980" windowWidth="31260" windowHeight="17280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -38,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="142">
   <si>
     <t>Senior</t>
   </si>
@@ -215,9 +210,6 @@
   </si>
   <si>
     <t>http://linkedin.com/in/curtisjhowell</t>
-  </si>
-  <si>
-    <t>Curtis is pursuing degrees in Informatics and Business Administration with a focus in Entrepreneurship. He keeps busy with a number of volunteer activities including serving student representative on the Student Technology Fee Committee for the University of Washington and as the IT Manager for Montlake Consulting Group. Last summer Curtis interned as a Program Manager with Microsoft Office before crossing the pond to study abroad for a semester at Copenhagen Business School. In his spare time, Curtis enjoys tennis, golf, softball, skiing and competing in triathlons.</t>
   </si>
   <si>
     <t>Eric</t>
@@ -462,6 +454,12 @@
   </si>
   <si>
     <t>http://www.linkedin.com/pub/mason-wrolstad/39/42/6b9</t>
+  </si>
+  <si>
+    <t>King County Metro, Windermere</t>
+  </si>
+  <si>
+    <t>Curtis is pursuing degrees in Informatics and Business Administration with a focus in Entrepreneurship. He keeps busy with a number of volunteer activities including serving as a student representative on the Student Technology Fee Committee for the University of Washington and as the IT Manager for Montlake Consulting Group. During the past two summers, Curtis was a Program Manager intern at Microsoft Office. In addition, he studied abroad at Copenhagen Business School for a semester in 2011. In his spare time, Curtis enjoys tennis, golf, softball, skiing and competing in triathlons.</t>
   </si>
 </sst>
 </file>
@@ -525,44 +523,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
-<MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
-  <Schema ID="Schema1">
-    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
-      <xsd:element nillable="true" name="people">
-        <xsd:complexType>
-          <xsd:sequence minOccurs="0">
-            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="person" form="unqualified">
-              <xsd:complexType>
-                <xsd:all>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="firstname" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="lastname" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="class" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="major1" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="concentration1" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="major2" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="bio" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="position" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="projects" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:anyURI" name="linkedin" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="imagethumb" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="concentration2" form="unqualified"/>
-                </xsd:all>
-              </xsd:complexType>
-            </xsd:element>
-          </xsd:sequence>
-        </xsd:complexType>
-      </xsd:element>
-    </xsd:schema>
-  </Schema>
-  <Map ID="1" Name="people_Map" RootElement="people" SchemaID="Schema1" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="3" DataBindingLoadMode="1"/>
-  </Map>
-</MapInfo>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:M28" tableType="xml" totalsRowShown="0" connectionId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:M28" tableType="xml" totalsRowShown="0">
   <sortState ref="B2:M28">
     <sortCondition ref="E2:E28" customList="Managing Partner,Junior Partner,Manager,Consultant"/>
     <sortCondition ref="C2:C28"/>
@@ -933,67 +895,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="29.625" customWidth="1"/>
-    <col min="2" max="2" width="11.875" customWidth="1"/>
-    <col min="3" max="3" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
-    <col min="5" max="5" width="34.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="81" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="44.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="44.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="56" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="1"/>
       <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
         <v>76</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>77</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" t="s">
         <v>78</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" t="s">
         <v>84</v>
       </c>
-      <c r="F1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H1" t="s">
-        <v>81</v>
-      </c>
-      <c r="I1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J1" t="s">
-        <v>83</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>85</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>86</v>
       </c>
-      <c r="M1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:13" ht="18" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
         <v>56</v>
@@ -1005,7 +967,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -1017,10 +979,10 @@
         <v>7</v>
       </c>
       <c r="J2" t="s">
-        <v>59</v>
+        <v>141</v>
       </c>
       <c r="K2" t="s">
-        <v>20</v>
+        <v>140</v>
       </c>
       <c r="L2" t="s">
         <v>58</v>
@@ -1030,7 +992,7 @@
         <v>CurtisH.jpg</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="18" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>35</v>
@@ -1042,7 +1004,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>37</v>
@@ -1053,7 +1015,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>39</v>
@@ -1066,7 +1028,7 @@
         <v>CoryS.jpg</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="18" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
         <v>26</v>
@@ -1078,7 +1040,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>5</v>
@@ -1100,13 +1062,13 @@
         <v>EvanG.jpg</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="18" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>0</v>
@@ -1127,18 +1089,18 @@
         <v>48</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M5" t="str">
         <f>CONCATENATE(Table1[[#This Row],[firstname]], LEFT(Table1[[#This Row],[lastname]],1),".jpg")</f>
         <v>EricB.jpg</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="18" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
         <v>51</v>
@@ -1165,7 +1127,7 @@
         <v>41</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2" t="s">
@@ -1176,7 +1138,7 @@
         <v>SuparnoC.jpg</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="18" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>31</v>
@@ -1203,7 +1165,7 @@
         <v>22</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2" t="s">
@@ -1214,7 +1176,7 @@
         <v>AdamG.jpg</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="18" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
         <v>16</v>
@@ -1239,7 +1201,7 @@
         <v>19</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>20</v>
@@ -1252,7 +1214,7 @@
         <v>JimI.jpg</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="18" customHeight="1">
       <c r="B9" s="2" t="s">
         <v>42</v>
       </c>
@@ -1274,7 +1236,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2" t="s">
@@ -1285,7 +1247,7 @@
         <v>MunirN.jpg</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="18" customHeight="1">
       <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
@@ -1307,7 +1269,7 @@
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -1316,7 +1278,7 @@
         <v>MichaelA.jpg</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="18" customHeight="1">
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1340,7 +1302,7 @@
         <v>14</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2" t="s">
@@ -1351,7 +1313,7 @@
         <v>RichA.jpg</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="18" customHeight="1">
       <c r="B12" s="2" t="s">
         <v>46</v>
       </c>
@@ -1384,12 +1346,12 @@
         <v>KyleB.jpg</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="18" customHeight="1">
       <c r="B13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>4</v>
@@ -1404,18 +1366,18 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M13" t="str">
         <f>CONCATENATE(Table1[[#This Row],[firstname]], LEFT(Table1[[#This Row],[lastname]],1),".jpg")</f>
         <v>WuenO.jpg</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="18" customHeight="1">
       <c r="B14" s="2" t="s">
         <v>2</v>
       </c>
@@ -1452,12 +1414,12 @@
         <v>TimT.jpg</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="18" customHeight="1">
       <c r="B15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" t="s">
         <v>90</v>
-      </c>
-      <c r="C15" t="s">
-        <v>91</v>
       </c>
       <c r="D15" t="s">
         <v>4</v>
@@ -1474,23 +1436,23 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M15" s="2" t="str">
         <f>CONCATENATE(Table1[[#This Row],[firstname]], LEFT(Table1[[#This Row],[lastname]],1),".jpg")</f>
         <v>CameronC.jpg</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="18" customHeight="1">
       <c r="B16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" t="s">
         <v>92</v>
-      </c>
-      <c r="C16" t="s">
-        <v>93</v>
       </c>
       <c r="D16" t="s">
         <v>4</v>
@@ -1507,23 +1469,23 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M16" s="2" t="str">
         <f>CONCATENATE(Table1[[#This Row],[firstname]], LEFT(Table1[[#This Row],[lastname]],1),".jpg")</f>
         <v>TomokiL.jpg</v>
       </c>
     </row>
-    <row r="17" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" ht="18" customHeight="1">
       <c r="B17" t="s">
         <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D17" t="s">
         <v>0</v>
@@ -1535,28 +1497,28 @@
         <v>5</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M17" s="2" t="str">
         <f>CONCATENATE(Table1[[#This Row],[firstname]], LEFT(Table1[[#This Row],[lastname]],1),".jpg")</f>
         <v>CurtisL.jpg</v>
       </c>
     </row>
-    <row r="18" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" ht="18" customHeight="1">
       <c r="B18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" t="s">
         <v>95</v>
-      </c>
-      <c r="C18" t="s">
-        <v>96</v>
       </c>
       <c r="D18" t="s">
         <v>4</v>
@@ -1576,12 +1538,12 @@
         <v>QuinnL.jpg</v>
       </c>
     </row>
-    <row r="19" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" ht="18" customHeight="1">
       <c r="B19" t="s">
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D19" t="s">
         <v>4</v>
@@ -1594,12 +1556,12 @@
         <v>MichaelM.jpg</v>
       </c>
     </row>
-    <row r="20" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" ht="18" customHeight="1">
       <c r="B20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" t="s">
         <v>98</v>
-      </c>
-      <c r="C20" t="s">
-        <v>99</v>
       </c>
       <c r="D20" t="s">
         <v>0</v>
@@ -1611,28 +1573,28 @@
         <v>5</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K20" s="2"/>
       <c r="L20" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M20" s="2" t="str">
         <f>CONCATENATE(Table1[[#This Row],[firstname]], LEFT(Table1[[#This Row],[lastname]],1),".jpg")</f>
         <v>JonathanM.jpg</v>
       </c>
     </row>
-    <row r="21" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" ht="18" customHeight="1">
       <c r="B21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D21" t="s">
         <v>4</v>
@@ -1641,31 +1603,31 @@
         <v>1</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K21" s="2"/>
       <c r="L21" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M21" s="2" t="str">
         <f>CONCATENATE(Table1[[#This Row],[firstname]], LEFT(Table1[[#This Row],[lastname]],1),".jpg")</f>
         <v>CameronN.jpg</v>
       </c>
     </row>
-    <row r="22" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" ht="18" customHeight="1">
       <c r="B22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" t="s">
         <v>101</v>
-      </c>
-      <c r="C22" t="s">
-        <v>102</v>
       </c>
       <c r="D22" t="s">
         <v>0</v>
@@ -1677,28 +1639,28 @@
         <v>7</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K22" s="2"/>
       <c r="L22" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M22" s="2" t="str">
         <f>CONCATENATE(Table1[[#This Row],[firstname]], LEFT(Table1[[#This Row],[lastname]],1),".jpg")</f>
         <v>ChaitraliP.jpg</v>
       </c>
     </row>
-    <row r="23" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" ht="18" customHeight="1">
       <c r="B23" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" t="s">
         <v>103</v>
-      </c>
-      <c r="C23" t="s">
-        <v>104</v>
       </c>
       <c r="D23" t="s">
         <v>4</v>
@@ -1710,28 +1672,28 @@
         <v>5</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M23" s="2" t="str">
         <f>CONCATENATE(Table1[[#This Row],[firstname]], LEFT(Table1[[#This Row],[lastname]],1),".jpg")</f>
         <v>JetS.jpg</v>
       </c>
     </row>
-    <row r="24" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" ht="18" customHeight="1">
       <c r="B24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" t="s">
         <v>113</v>
-      </c>
-      <c r="C24" t="s">
-        <v>114</v>
       </c>
       <c r="D24" t="s">
         <v>0</v>
@@ -1751,12 +1713,12 @@
         <v>CatrionaS.jpg</v>
       </c>
     </row>
-    <row r="25" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" ht="18" customHeight="1">
       <c r="B25" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" t="s">
         <v>105</v>
-      </c>
-      <c r="C25" t="s">
-        <v>106</v>
       </c>
       <c r="D25" t="s">
         <v>4</v>
@@ -1773,7 +1735,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
@@ -1782,12 +1744,12 @@
         <v>BrennenS.jpg</v>
       </c>
     </row>
-    <row r="26" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" ht="18" customHeight="1">
       <c r="B26" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" t="s">
         <v>107</v>
-      </c>
-      <c r="C26" t="s">
-        <v>108</v>
       </c>
       <c r="D26" t="s">
         <v>4</v>
@@ -1796,7 +1758,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>19</v>
@@ -1804,7 +1766,7 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
@@ -1813,12 +1775,12 @@
         <v>NashuaS.jpg</v>
       </c>
     </row>
-    <row r="27" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" ht="18" customHeight="1">
       <c r="B27" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" t="s">
         <v>109</v>
-      </c>
-      <c r="C27" t="s">
-        <v>110</v>
       </c>
       <c r="D27" t="s">
         <v>0</v>
@@ -1837,23 +1799,23 @@
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K27" s="2"/>
       <c r="L27" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M27" s="2" t="str">
         <f>CONCATENATE(Table1[[#This Row],[firstname]], LEFT(Table1[[#This Row],[lastname]],1),".jpg")</f>
         <v>MaiaS.jpg</v>
       </c>
     </row>
-    <row r="28" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13" ht="18" customHeight="1">
       <c r="B28" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" t="s">
         <v>111</v>
-      </c>
-      <c r="C28" t="s">
-        <v>112</v>
       </c>
       <c r="D28" t="s">
         <v>0</v>
@@ -1870,11 +1832,11 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M28" t="str">
         <f>CONCATENATE(Table1[[#This Row],[firstname]], LEFT(Table1[[#This Row],[lastname]],1),".jpg")</f>

</xml_diff>